<commit_message>
Debugging nasty FNF error
</commit_message>
<xml_diff>
--- a/Data/ClueLayoutColored.xlsx
+++ b/Data/ClueLayoutColored.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da3873474e39d809/Desktop/ClueGame/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec2c82c9f3cbf5bf/Documents/GitHub/ClueGame/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="466" documentId="8_{10C72155-1E25-4505-BAD9-74605B4415FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C679A54-B371-4953-8C5D-46AABE289F30}"/>
+  <xr:revisionPtr revIDLastSave="468" documentId="8_{10C72155-1E25-4505-BAD9-74605B4415FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EA4CC3A-8400-469C-B685-88B0BC8F4CF6}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{61EB29D2-5BBF-4C24-8184-1513E291ED5C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{61EB29D2-5BBF-4C24-8184-1513E291ED5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Medium Board" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,7 +328,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -346,7 +346,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +361,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -687,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647A6E94-35CE-47C0-8BFB-0D328AC3C2AF}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,7 +966,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>7</v>
@@ -1001,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>3</v>
@@ -1426,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71BD2320-D59C-4FE3-962A-D194E7A3AA69}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2160,169 +2155,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="14"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" s="20"/>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" s="14"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>